<commit_message>
timer plaatjes met superzuig as
</commit_message>
<xml_diff>
--- a/verslaglegging en presentaties/testruns 2017-18-05.xlsx
+++ b/verslaglegging en presentaties/testruns 2017-18-05.xlsx
@@ -19,10 +19,11 @@
     <sheet name="len8" sheetId="4" r:id="rId5"/>
     <sheet name="len9" sheetId="5" r:id="rId6"/>
     <sheet name="len10" sheetId="6" r:id="rId7"/>
+    <sheet name="len15" sheetId="8" r:id="rId8"/>
+    <sheet name="len20" sheetId="9" r:id="rId9"/>
+    <sheet name="len25" sheetId="10" r:id="rId10"/>
+    <sheet name="len30" sheetId="11" r:id="rId11"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="8">
   <si>
     <t>Depth0</t>
   </si>
@@ -226,10 +227,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Averages!$A$2:$A$7</c:f>
+              <c:f>Averages!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -247,6 +248,18 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -297,10 +310,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Averages!$A$2:$A$7</c:f>
+              <c:f>Averages!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -318,6 +331,18 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -368,10 +393,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Averages!$A$2:$A$7</c:f>
+              <c:f>Averages!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -389,6 +414,18 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -442,10 +479,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Averages!$A$2:$A$7</c:f>
+              <c:f>Averages!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -463,16 +500,28 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Averages!$E$2:$E$7</c:f>
+              <c:f>Averages!$E$2:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1E-4</c:v>
                 </c:pt>
@@ -490,6 +539,18 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3.7000000000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16880000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.21090000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4264</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -505,8 +566,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="642384272"/>
-        <c:axId val="642378832"/>
+        <c:axId val="-1833411568"/>
+        <c:axId val="-1833411024"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
@@ -533,13 +594,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Averages!$A$2:$A$7</c15:sqref>
+                          <c15:sqref>Averages!$A$2:$A$11</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="6"/>
+                      <c:ptCount val="10"/>
                       <c:pt idx="0">
                         <c:v>5</c:v>
                       </c:pt>
@@ -557,6 +618,18 @@
                       </c:pt>
                       <c:pt idx="5">
                         <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>20</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>30</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -601,7 +674,7 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="642384272"/>
+        <c:axId val="-1833411568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -700,7 +773,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="642378832"/>
+        <c:crossAx val="-1833411024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -708,7 +781,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="642378832"/>
+        <c:axId val="-1833411024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -814,7 +887,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="642384272"/>
+        <c:crossAx val="-1833411568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1456,15 +1529,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>45720</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>388620</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1484,116 +1557,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="totals"/>
-      <sheetName val="len6"/>
-      <sheetName val="len7"/>
-      <sheetName val="len8"/>
-      <sheetName val="len9"/>
-      <sheetName val="len10"/>
-      <sheetName val="len11"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2">
-            <v>6</v>
-          </cell>
-          <cell r="C2">
-            <v>0</v>
-          </cell>
-          <cell r="D2">
-            <v>0</v>
-          </cell>
-          <cell r="E2">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>7</v>
-          </cell>
-          <cell r="C3">
-            <v>4.200000000000001E-2</v>
-          </cell>
-          <cell r="D3">
-            <v>1.9200000000000002E-2</v>
-          </cell>
-          <cell r="E3">
-            <v>1.6000000000000001E-3</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>8</v>
-          </cell>
-          <cell r="C4">
-            <v>0.186</v>
-          </cell>
-          <cell r="D4">
-            <v>6.5799999999999997E-2</v>
-          </cell>
-          <cell r="E4">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>9</v>
-          </cell>
-          <cell r="C5">
-            <v>2.0714000000000001</v>
-          </cell>
-          <cell r="D5">
-            <v>0.84689999999999999</v>
-          </cell>
-          <cell r="E5">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>10</v>
-          </cell>
-          <cell r="C6">
-            <v>20.572300000000002</v>
-          </cell>
-          <cell r="D6">
-            <v>7.5368000000000013</v>
-          </cell>
-          <cell r="E6">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>11</v>
-          </cell>
-          <cell r="C7">
-            <v>132.62619999999998</v>
-          </cell>
-          <cell r="D7">
-            <v>42.049400000000006</v>
-          </cell>
-          <cell r="E7">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1859,10 +1822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2032,9 +1995,279 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="E8">
+        <f>'len15'!E$12</f>
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <f>'len20'!E$12</f>
+        <v>0.16880000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <f>'len25'!E$12</f>
+        <v>0.21090000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <f>'len30'!E$12</f>
+        <v>0.4264</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A1:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>0.219</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="E6">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>0.25</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>0.219</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:F12" si="0">AVERAGE(E2:E11, E14:E16)</f>
+        <v>0.21090000000000003</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>0.438</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="E6">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:F12" si="0">AVERAGE(E2:E11, E14:E16)</f>
+        <v>0.4264</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3230,7 +3463,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A12" sqref="A1:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3362,12 +3595,246 @@
         <v>5</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="C12:F12" si="0">AVERAGE(D2:D11, D14:D16)</f>
+        <f t="shared" ref="D12:F12" si="0">AVERAGE(D2:D11, D14:D16)</f>
         <v>108.60840000000003</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
         <v>3.7000000000000006E-3</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A1:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>3.1E-2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="E6">
+        <v>3.1E-2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>3.1E-2</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>3.1E-2</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="D12:F12" si="0">AVERAGE(E2:E11, E14:E16)</f>
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A1:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>6.2E-2</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="E6">
+        <v>0.94</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>0.109</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>0.109</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:F12" si="0">AVERAGE(E2:E11, E14:E16)</f>
+        <v>0.16880000000000001</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>

</xml_diff>